<commit_message>
Fix règle de gestion 87c864fd83c91f4ff17a7fb557addea6401752a9
</commit_message>
<xml_diff>
--- a/issues96/ig/StructureDefinition-sdo-task.xlsx
+++ b/issues96/ig/StructureDefinition-sdo-task.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-26T11:08:19+00:00</t>
+    <t>2024-03-28T15:28:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -263,7 +263,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}inv-1:Last modified date must be greater than or equal to authored-on date. {lastModified.exists().not() or authoredOn.exists().not() or lastModified &gt;= authoredOn}regle-StatutUnite:Si statut unite est rempli alors les éléments suivants sont attendus :idUnite,nomUnite, categorieOrganisation, modePriseCharge, dateStatutUnite {(input.type.where(text='idUnite').exists()) implies (input.type.where(text='nomUnite').exists() and input.type.where(text='categorieOrganisation').exists() and input.type.where(text='modePriseCharge').exists() and input.type.where(text='dateStatutUnite').exists() and input.type.where(text='statutUnite').exists())}regle-ModePriseEnCharge:Les codes possibles pour le mode de prise en charge sont : Code 46 « Hébergement (accueil jour et nuit) » = Internat (1),Code 47 « Accueil de jour » = externat (2), semi-internat (3) ou accueil de jour (6),Code 48 Accueil de nuit » = Accueil de nuit (4) {input.where(type.text='modePriseCharge').value.coding.code='48' or input.where(type.text='modePriseCharge').value.coding.code='47'  or input.where(type.text='modePriseCharge').value.coding.code='46' or input.where(type.text='modePriseCharge').exists().not() }</t>
+dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}inv-1:Last modified date must be greater than or equal to authored-on date. {lastModified.exists().not() or authoredOn.exists().not() or lastModified &gt;= authoredOn}regle-StatutUnite:Si statut unite est rempli alors les éléments suivants sont attendus :idUnite,nomUnite, categorieOrganisation, modePriseCharge, dateStatutUnite {(input.type.where(text='statutUnite').exists()) implies (input.type.where(text='nomUnite').exists() and input.type.where(text='categorieOrganisation').exists() and input.type.where(text='modePriseCharge').exists() and input.type.where(text='dateStatutUnite').exists() and input.type.where(text='idUnite').exists())}regle-ModePriseEnCharge:Les codes possibles pour le mode de prise en charge sont : Code 46 « Hébergement (accueil jour et nuit) » = Internat (1),Code 47 « Accueil de jour » = externat (2), semi-internat (3) ou accueil de jour (6),Code 48 Accueil de nuit » = Accueil de nuit (4) {input.where(type.text='modePriseCharge').value.coding.code='48' or input.where(type.text='modePriseCharge').value.coding.code='47'  or input.where(type.text='modePriseCharge').value.coding.code='46' or input.where(type.text='modePriseCharge').exists().not() }</t>
   </si>
   <si>
     <t>Request, Event</t>

</xml_diff>

<commit_message>
Fix Regle gestion Task c57ef94b38cab8b071191e440298167524c6e7dd
</commit_message>
<xml_diff>
--- a/issues96/ig/StructureDefinition-sdo-task.xlsx
+++ b/issues96/ig/StructureDefinition-sdo-task.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6074" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6074" uniqueCount="651">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-28T15:28:05+00:00</t>
+    <t>2024-04-02T07:24:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -263,7 +263,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}inv-1:Last modified date must be greater than or equal to authored-on date. {lastModified.exists().not() or authoredOn.exists().not() or lastModified &gt;= authoredOn}regle-StatutUnite:Si statut unite est rempli alors les éléments suivants sont attendus :idUnite,nomUnite, categorieOrganisation, modePriseCharge, dateStatutUnite {(input.type.where(text='statutUnite').exists()) implies (input.type.where(text='nomUnite').exists() and input.type.where(text='categorieOrganisation').exists() and input.type.where(text='modePriseCharge').exists() and input.type.where(text='dateStatutUnite').exists() and input.type.where(text='idUnite').exists())}regle-ModePriseEnCharge:Les codes possibles pour le mode de prise en charge sont : Code 46 « Hébergement (accueil jour et nuit) » = Internat (1),Code 47 « Accueil de jour » = externat (2), semi-internat (3) ou accueil de jour (6),Code 48 Accueil de nuit » = Accueil de nuit (4) {input.where(type.text='modePriseCharge').value.coding.code='48' or input.where(type.text='modePriseCharge').value.coding.code='47'  or input.where(type.text='modePriseCharge').value.coding.code='46' or input.where(type.text='modePriseCharge').exists().not() }</t>
+dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}inv-1:Last modified date must be greater than or equal to authored-on date. {lastModified.exists().not() or authoredOn.exists().not() or lastModified &gt;= authoredOn}regle-StatutUnite:Si statut unite est rempli alors les éléments suivants sont attendus :idUnite,nomUnite, categorieOrganisation, modePriseCharge, dateStatutUnite {(input.type.where(text='statutUnite').exists()) implies (input.type.where(text='nomUnite').exists() and input.type.where(text='categorieOrganisation').exists() and input.type.where(text='modePriseCharge').exists() and input.type.where(text='dateStatutUnite').exists() and input.type.where(text='idUnite').exists())}</t>
   </si>
   <si>
     <t>Request, Event</t>
@@ -1582,7 +1582,7 @@
     <t>motifESMS</t>
   </si>
   <si>
-    <t>Permet de définir le motif associé au statut de l’usager dans l’ESMS. Motifs obligatoires pour certains statuts suivant la table : https://mos.esante.gouv.fr/NOS/ASS_A32-StatutMotifPersonnePriseCharge/ASS_A32-StatutMotifPersonnePriseCharge.pdf</t>
+    <t>Permet de définir le motif associé au statut de l’usager dans l’ESMS.</t>
   </si>
   <si>
     <t>Task.input:motifESMS.id</t>
@@ -1608,6 +1608,9 @@
     <t>Task.input:motifESMS.value[x]</t>
   </si>
   <si>
+    <t xml:space="preserve"> Motifs obligatoires pour certains statuts suivant la table : https://mos.esante.gouv.fr/NOS/ASS_A32-StatutMotifPersonnePriseCharge/ASS_A32-StatutMotifPersonnePriseCharge.pdf</t>
+  </si>
+  <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J251-MotifStatutPersonnePriseChargeESMS/FHIR/JDV-J251-MotifStatutPersonnePriseChargeESMS</t>
   </si>
   <si>
@@ -1824,6 +1827,10 @@
   </si>
   <si>
     <t>Permet de définir le mode de prise en charge</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+regle-ModePriseEnCharge:Les codes possibles pour le mode de prise en charge sont : 46 (Hébergement (accueil jour et nuit)) ; 47 (Accueil de jour); 48 (Accueil de nuit) {value.coding.code='48' or value.coding.code='47' or value.coding.code='46'}</t>
   </si>
   <si>
     <t>Task.input:modePriseCharge.id</t>
@@ -11873,7 +11880,7 @@
         <v>251</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>467</v>
+        <v>506</v>
       </c>
       <c r="M83" t="s" s="2">
         <v>468</v>
@@ -11907,7 +11914,7 @@
       </c>
       <c r="Y83" s="2"/>
       <c r="Z83" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>76</v>
@@ -11954,13 +11961,13 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B84" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C84" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D84" t="s" s="2">
         <v>448</v>
@@ -11985,7 +11992,7 @@
         <v>417</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="M84" t="s" s="2">
         <v>451</v>
@@ -12070,7 +12077,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B85" t="s" s="2">
         <v>455</v>
@@ -12182,7 +12189,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B86" t="s" s="2">
         <v>456</v>
@@ -12296,7 +12303,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B87" t="s" s="2">
         <v>457</v>
@@ -12412,7 +12419,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B88" t="s" s="2">
         <v>458</v>
@@ -12460,7 +12467,7 @@
         <v>76</v>
       </c>
       <c r="S88" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="T88" t="s" s="2">
         <v>76</v>
@@ -12528,7 +12535,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B89" t="s" s="2">
         <v>465</v>
@@ -12554,7 +12561,7 @@
         <v>76</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L89" t="s" s="2">
         <v>467</v>
@@ -12640,13 +12647,13 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B90" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C90" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D90" t="s" s="2">
         <v>448</v>
@@ -12671,7 +12678,7 @@
         <v>417</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="M90" t="s" s="2">
         <v>451</v>
@@ -12756,7 +12763,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B91" t="s" s="2">
         <v>455</v>
@@ -12868,7 +12875,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B92" t="s" s="2">
         <v>456</v>
@@ -12982,7 +12989,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B93" t="s" s="2">
         <v>457</v>
@@ -13098,7 +13105,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B94" t="s" s="2">
         <v>458</v>
@@ -13146,7 +13153,7 @@
         <v>76</v>
       </c>
       <c r="S94" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="T94" t="s" s="2">
         <v>76</v>
@@ -13214,7 +13221,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B95" t="s" s="2">
         <v>465</v>
@@ -13326,13 +13333,13 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B96" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C96" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D96" t="s" s="2">
         <v>448</v>
@@ -13357,7 +13364,7 @@
         <v>417</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M96" t="s" s="2">
         <v>451</v>
@@ -13442,7 +13449,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B97" t="s" s="2">
         <v>455</v>
@@ -13554,7 +13561,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B98" t="s" s="2">
         <v>456</v>
@@ -13668,7 +13675,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B99" t="s" s="2">
         <v>457</v>
@@ -13784,7 +13791,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B100" t="s" s="2">
         <v>458</v>
@@ -13832,7 +13839,7 @@
         <v>76</v>
       </c>
       <c r="S100" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="T100" t="s" s="2">
         <v>76</v>
@@ -13900,7 +13907,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B101" t="s" s="2">
         <v>465</v>
@@ -14012,13 +14019,13 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B102" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C102" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D102" t="s" s="2">
         <v>448</v>
@@ -14043,7 +14050,7 @@
         <v>417</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M102" t="s" s="2">
         <v>451</v>
@@ -14128,7 +14135,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B103" t="s" s="2">
         <v>455</v>
@@ -14240,7 +14247,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B104" t="s" s="2">
         <v>456</v>
@@ -14354,7 +14361,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B105" t="s" s="2">
         <v>457</v>
@@ -14470,7 +14477,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B106" t="s" s="2">
         <v>458</v>
@@ -14518,7 +14525,7 @@
         <v>76</v>
       </c>
       <c r="S106" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="T106" t="s" s="2">
         <v>76</v>
@@ -14586,7 +14593,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B107" t="s" s="2">
         <v>465</v>
@@ -14649,7 +14656,7 @@
       </c>
       <c r="Y107" s="2"/>
       <c r="Z107" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AA107" t="s" s="2">
         <v>76</v>
@@ -14696,13 +14703,13 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B108" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C108" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D108" t="s" s="2">
         <v>448</v>
@@ -14727,7 +14734,7 @@
         <v>417</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="M108" t="s" s="2">
         <v>451</v>
@@ -14812,7 +14819,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B109" t="s" s="2">
         <v>455</v>
@@ -14924,7 +14931,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B110" t="s" s="2">
         <v>456</v>
@@ -15038,7 +15045,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B111" t="s" s="2">
         <v>457</v>
@@ -15154,7 +15161,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B112" t="s" s="2">
         <v>458</v>
@@ -15202,7 +15209,7 @@
         <v>76</v>
       </c>
       <c r="S112" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="T112" t="s" s="2">
         <v>76</v>
@@ -15270,7 +15277,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B113" t="s" s="2">
         <v>465</v>
@@ -15333,7 +15340,7 @@
       </c>
       <c r="Y113" s="2"/>
       <c r="Z113" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AA113" t="s" s="2">
         <v>76</v>
@@ -15380,13 +15387,13 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B114" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C114" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D114" t="s" s="2">
         <v>448</v>
@@ -15411,7 +15418,7 @@
         <v>417</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="M114" t="s" s="2">
         <v>451</v>
@@ -15496,7 +15503,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B115" t="s" s="2">
         <v>455</v>
@@ -15608,7 +15615,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B116" t="s" s="2">
         <v>456</v>
@@ -15722,7 +15729,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B117" t="s" s="2">
         <v>457</v>
@@ -15838,7 +15845,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B118" t="s" s="2">
         <v>458</v>
@@ -15886,7 +15893,7 @@
         <v>76</v>
       </c>
       <c r="S118" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="T118" t="s" s="2">
         <v>76</v>
@@ -15954,7 +15961,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B119" t="s" s="2">
         <v>465</v>
@@ -15980,7 +15987,7 @@
         <v>76</v>
       </c>
       <c r="K119" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="L119" t="s" s="2">
         <v>467</v>
@@ -16066,13 +16073,13 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B120" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C120" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D120" t="s" s="2">
         <v>448</v>
@@ -16097,7 +16104,7 @@
         <v>417</v>
       </c>
       <c r="L120" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="M120" t="s" s="2">
         <v>451</v>
@@ -16165,7 +16172,7 @@
         <v>98</v>
       </c>
       <c r="AJ120" t="s" s="2">
-        <v>99</v>
+        <v>569</v>
       </c>
       <c r="AK120" t="s" s="2">
         <v>76</v>
@@ -16182,7 +16189,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="2">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B121" t="s" s="2">
         <v>455</v>
@@ -16294,7 +16301,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B122" t="s" s="2">
         <v>456</v>
@@ -16408,7 +16415,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B123" t="s" s="2">
         <v>457</v>
@@ -16524,7 +16531,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B124" t="s" s="2">
         <v>458</v>
@@ -16572,7 +16579,7 @@
         <v>76</v>
       </c>
       <c r="S124" t="s" s="2">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="T124" t="s" s="2">
         <v>76</v>
@@ -16640,7 +16647,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B125" t="s" s="2">
         <v>465</v>
@@ -16703,7 +16710,7 @@
       </c>
       <c r="Y125" s="2"/>
       <c r="Z125" t="s" s="2">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="AA125" t="s" s="2">
         <v>76</v>
@@ -16750,13 +16757,13 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B126" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C126" t="s" s="2">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D126" t="s" s="2">
         <v>448</v>
@@ -16781,7 +16788,7 @@
         <v>417</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="M126" t="s" s="2">
         <v>451</v>
@@ -16866,7 +16873,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B127" t="s" s="2">
         <v>455</v>
@@ -16978,7 +16985,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B128" t="s" s="2">
         <v>456</v>
@@ -17092,7 +17099,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B129" t="s" s="2">
         <v>457</v>
@@ -17208,7 +17215,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="B130" t="s" s="2">
         <v>458</v>
@@ -17256,7 +17263,7 @@
         <v>76</v>
       </c>
       <c r="S130" t="s" s="2">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="T130" t="s" s="2">
         <v>76</v>
@@ -17324,7 +17331,7 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B131" t="s" s="2">
         <v>465</v>
@@ -17387,7 +17394,7 @@
       </c>
       <c r="Y131" s="2"/>
       <c r="Z131" t="s" s="2">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="AA131" t="s" s="2">
         <v>76</v>
@@ -17434,13 +17441,13 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B132" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C132" t="s" s="2">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D132" t="s" s="2">
         <v>448</v>
@@ -17465,7 +17472,7 @@
         <v>417</v>
       </c>
       <c r="L132" t="s" s="2">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="M132" t="s" s="2">
         <v>451</v>
@@ -17550,7 +17557,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B133" t="s" s="2">
         <v>455</v>
@@ -17662,7 +17669,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B134" t="s" s="2">
         <v>456</v>
@@ -17776,7 +17783,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B135" t="s" s="2">
         <v>457</v>
@@ -17892,7 +17899,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B136" t="s" s="2">
         <v>458</v>
@@ -17940,7 +17947,7 @@
         <v>76</v>
       </c>
       <c r="S136" t="s" s="2">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="T136" t="s" s="2">
         <v>76</v>
@@ -18008,7 +18015,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B137" t="s" s="2">
         <v>465</v>
@@ -18034,7 +18041,7 @@
         <v>76</v>
       </c>
       <c r="K137" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L137" t="s" s="2">
         <v>467</v>
@@ -18120,13 +18127,13 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B138" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C138" t="s" s="2">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D138" t="s" s="2">
         <v>448</v>
@@ -18151,7 +18158,7 @@
         <v>417</v>
       </c>
       <c r="L138" t="s" s="2">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="M138" t="s" s="2">
         <v>451</v>
@@ -18236,7 +18243,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B139" t="s" s="2">
         <v>455</v>
@@ -18348,7 +18355,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B140" t="s" s="2">
         <v>456</v>
@@ -18462,7 +18469,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B141" t="s" s="2">
         <v>457</v>
@@ -18578,7 +18585,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B142" t="s" s="2">
         <v>458</v>
@@ -18626,7 +18633,7 @@
         <v>76</v>
       </c>
       <c r="S142" t="s" s="2">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="T142" t="s" s="2">
         <v>76</v>
@@ -18694,7 +18701,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B143" t="s" s="2">
         <v>465</v>
@@ -18723,7 +18730,7 @@
         <v>251</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="M143" t="s" s="2">
         <v>468</v>
@@ -18757,7 +18764,7 @@
       </c>
       <c r="Y143" s="2"/>
       <c r="Z143" t="s" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="AA143" t="s" s="2">
         <v>76</v>
@@ -18804,13 +18811,13 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="2">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B144" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C144" t="s" s="2">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D144" t="s" s="2">
         <v>448</v>
@@ -18835,7 +18842,7 @@
         <v>417</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="M144" t="s" s="2">
         <v>451</v>
@@ -18920,7 +18927,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="2">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B145" t="s" s="2">
         <v>455</v>
@@ -19032,7 +19039,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="2">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B146" t="s" s="2">
         <v>456</v>
@@ -19146,7 +19153,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="2">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B147" t="s" s="2">
         <v>457</v>
@@ -19262,7 +19269,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s" s="2">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B148" t="s" s="2">
         <v>458</v>
@@ -19310,7 +19317,7 @@
         <v>76</v>
       </c>
       <c r="S148" t="s" s="2">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="T148" t="s" s="2">
         <v>76</v>
@@ -19378,7 +19385,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B149" t="s" s="2">
         <v>465</v>
@@ -19441,7 +19448,7 @@
       </c>
       <c r="Y149" s="2"/>
       <c r="Z149" t="s" s="2">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="AA149" t="s" s="2">
         <v>76</v>
@@ -19488,13 +19495,13 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B150" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C150" t="s" s="2">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D150" t="s" s="2">
         <v>448</v>
@@ -19519,7 +19526,7 @@
         <v>417</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="M150" t="s" s="2">
         <v>451</v>
@@ -19604,7 +19611,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s" s="2">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B151" t="s" s="2">
         <v>455</v>
@@ -19716,7 +19723,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s" s="2">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B152" t="s" s="2">
         <v>456</v>
@@ -19830,7 +19837,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="2">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B153" t="s" s="2">
         <v>457</v>
@@ -19946,7 +19953,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="2">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B154" t="s" s="2">
         <v>458</v>
@@ -19994,7 +20001,7 @@
         <v>76</v>
       </c>
       <c r="S154" t="s" s="2">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="T154" t="s" s="2">
         <v>76</v>
@@ -20062,7 +20069,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="2">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B155" t="s" s="2">
         <v>465</v>
@@ -20174,13 +20181,13 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="2">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B156" t="s" s="2">
         <v>447</v>
       </c>
       <c r="C156" t="s" s="2">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D156" t="s" s="2">
         <v>448</v>
@@ -20205,7 +20212,7 @@
         <v>417</v>
       </c>
       <c r="L156" t="s" s="2">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="M156" t="s" s="2">
         <v>451</v>
@@ -20290,7 +20297,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s" s="2">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B157" t="s" s="2">
         <v>455</v>
@@ -20402,7 +20409,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B158" t="s" s="2">
         <v>456</v>
@@ -20516,7 +20523,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B159" t="s" s="2">
         <v>457</v>
@@ -20632,7 +20639,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B160" t="s" s="2">
         <v>458</v>
@@ -20680,7 +20687,7 @@
         <v>76</v>
       </c>
       <c r="S160" t="s" s="2">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="T160" t="s" s="2">
         <v>76</v>
@@ -20748,7 +20755,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s" s="2">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B161" t="s" s="2">
         <v>465</v>
@@ -20860,10 +20867,10 @@
     </row>
     <row r="162">
       <c r="A162" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B162" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" t="s" s="2">
@@ -20889,14 +20896,14 @@
         <v>417</v>
       </c>
       <c r="L162" t="s" s="2">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="M162" t="s" s="2">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="N162" s="2"/>
       <c r="O162" t="s" s="2">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="P162" t="s" s="2">
         <v>76</v>
@@ -20945,7 +20952,7 @@
         <v>76</v>
       </c>
       <c r="AF162" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="AG162" t="s" s="2">
         <v>77</v>
@@ -20974,10 +20981,10 @@
     </row>
     <row r="163">
       <c r="A163" t="s" s="2">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B163" t="s" s="2">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" t="s" s="2">
@@ -21086,10 +21093,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B164" t="s" s="2">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" t="s" s="2">
@@ -21200,10 +21207,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B165" t="s" s="2">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" t="s" s="2">
@@ -21316,10 +21323,10 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="2">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B166" t="s" s="2">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" t="s" s="2">
@@ -21345,16 +21352,16 @@
         <v>251</v>
       </c>
       <c r="L166" t="s" s="2">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="M166" t="s" s="2">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="N166" t="s" s="2">
         <v>261</v>
       </c>
       <c r="O166" t="s" s="2">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="P166" t="s" s="2">
         <v>76</v>
@@ -21382,7 +21389,7 @@
         <v>156</v>
       </c>
       <c r="Y166" t="s" s="2">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="Z166" t="s" s="2">
         <v>76</v>
@@ -21403,7 +21410,7 @@
         <v>76</v>
       </c>
       <c r="AF166" t="s" s="2">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="AG166" t="s" s="2">
         <v>86</v>
@@ -21432,10 +21439,10 @@
     </row>
     <row r="167">
       <c r="A167" t="s" s="2">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B167" t="s" s="2">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C167" s="2"/>
       <c r="D167" t="s" s="2">
@@ -21461,14 +21468,14 @@
         <v>466</v>
       </c>
       <c r="L167" t="s" s="2">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="M167" t="s" s="2">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="N167" s="2"/>
       <c r="O167" t="s" s="2">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="P167" t="s" s="2">
         <v>76</v>
@@ -21517,7 +21524,7 @@
         <v>76</v>
       </c>
       <c r="AF167" t="s" s="2">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="AG167" t="s" s="2">
         <v>86</v>

</xml_diff>